<commit_message>
docs(Updated Smart Scheduling README)
</commit_message>
<xml_diff>
--- a/Smart Scheduling Challenge/Staff Schedule.xlsx
+++ b/Smart Scheduling Challenge/Staff Schedule.xlsx
@@ -886,22 +886,22 @@
         <v>45474.625</v>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1482,22 +1482,22 @@
         <v>45475.54166666666</v>
       </c>
       <c r="B39" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" t="n">
         <v>2</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="G39" t="n">
-        <v>3.142857142857143</v>
+        <v>3</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -1538,22 +1538,22 @@
         <v>45475.625</v>
       </c>
       <c r="B41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" t="n">
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G41" t="n">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -2218,7 +2218,7 @@
         <v>45476.66666666666</v>
       </c>
       <c r="B66" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66" t="n">
         <v>1</v>
@@ -2233,7 +2233,7 @@
         <v>4</v>
       </c>
       <c r="G66" t="n">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -2814,22 +2814,22 @@
         <v>45477.58333333334</v>
       </c>
       <c r="B88" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C88" t="n">
         <v>1</v>
       </c>
       <c r="D88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F88" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G88" t="n">
-        <v>2.5</v>
+        <v>3.142857142857143</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
@@ -2954,7 +2954,7 @@
         <v>45477.79166666666</v>
       </c>
       <c r="B93" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C93" t="n">
         <v>1</v>
@@ -2969,7 +2969,7 @@
         <v>4</v>
       </c>
       <c r="G93" t="n">
-        <v>5.5</v>
+        <v>5.25</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
@@ -3412,22 +3412,22 @@
         <v>45478.5</v>
       </c>
       <c r="B110" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C110" t="n">
         <v>1</v>
       </c>
       <c r="D110" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E110" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F110" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G110" t="n">
-        <v>2.5</v>
+        <v>3.142857142857143</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
@@ -3440,22 +3440,22 @@
         <v>45478.54166666666</v>
       </c>
       <c r="B111" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C111" t="n">
         <v>1</v>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E111" t="n">
         <v>1</v>
       </c>
       <c r="F111" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G111" t="n">
-        <v>4.333333333333333</v>
+        <v>3.5</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
@@ -4038,7 +4038,7 @@
         <v>45479.45833333334</v>
       </c>
       <c r="B133" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C133" t="n">
         <v>1</v>
@@ -4053,7 +4053,7 @@
         <v>4</v>
       </c>
       <c r="G133" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H133" t="inlineStr">
         <is>
@@ -4066,22 +4066,22 @@
         <v>45479.5</v>
       </c>
       <c r="B134" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C134" t="n">
         <v>1</v>
       </c>
       <c r="D134" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E134" t="n">
         <v>1</v>
       </c>
       <c r="F134" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G134" t="n">
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
@@ -4094,22 +4094,22 @@
         <v>45479.54166666666</v>
       </c>
       <c r="B135" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C135" t="n">
         <v>1</v>
       </c>
       <c r="D135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E135" t="n">
         <v>1</v>
       </c>
       <c r="F135" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G135" t="n">
-        <v>4.333333333333333</v>
+        <v>3.5</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
@@ -4122,22 +4122,22 @@
         <v>45479.58333333334</v>
       </c>
       <c r="B136" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C136" t="n">
         <v>1</v>
       </c>
       <c r="D136" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F136" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G136" t="n">
-        <v>2.5</v>
+        <v>3.142857142857143</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
@@ -4720,22 +4720,22 @@
         <v>45480.5</v>
       </c>
       <c r="B158" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C158" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D158" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E158" t="n">
         <v>0</v>
       </c>
       <c r="F158" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G158" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H158" t="inlineStr">
         <is>
@@ -4748,22 +4748,22 @@
         <v>45480.54166666666</v>
       </c>
       <c r="B159" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C159" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D159" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F159" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G159" t="n">
-        <v>3</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="H159" t="inlineStr">
         <is>

</xml_diff>